<commit_message>
Issue No.2 was partially resolved. Still some sub-motifs are acquired from delta analysis. Should be removed.
</commit_message>
<xml_diff>
--- a/Thesis code/Solutions/solutionsModified.xlsx
+++ b/Thesis code/Solutions/solutionsModified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renanabenyehuda/PycharmProjects/ThesisAlgorithm/Thesis code/Solutions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF47662-684A-6F4E-93C6-A56964930975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D370A7-D51F-B142-BAA5-6B7E55A45AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15320" yWindow="740" windowWidth="14920" windowHeight="18900" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15320" yWindow="760" windowWidth="14920" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#0" sheetId="1" r:id="rId1"/>
@@ -1212,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3397,7 +3397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>

</xml_diff>